<commit_message>
Hydrate cmd line pattern
</commit_message>
<xml_diff>
--- a/Grep Options Analysis.xlsx
+++ b/Grep Options Analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>b</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>treat file as binary</t>
+  </si>
+  <si>
+    <t>recursive+symlink</t>
   </si>
 </sst>
 </file>
@@ -808,7 +811,7 @@
   <dimension ref="B2:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1117,7 +1120,7 @@
         <v>41</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F27" s="18"/>
     </row>

</xml_diff>

<commit_message>
add -l (--files-with-matches) option
</commit_message>
<xml_diff>
--- a/Grep Options Analysis.xlsx
+++ b/Grep Options Analysis.xlsx
@@ -403,7 +403,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +452,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -489,17 +495,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -508,19 +508,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -528,6 +519,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,7 +819,7 @@
   <dimension ref="B2:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -823,10 +831,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="2:8">
       <c r="C3" s="2" t="s">
@@ -835,28 +843,28 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="21"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="9" spans="2:8">
       <c r="H9" t="s">
@@ -864,68 +872,68 @@
       </c>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="15" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="H12" s="20" t="s">
+      <c r="F12" s="13"/>
+      <c r="H12" s="15" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="17" t="s">
         <v>93</v>
       </c>
       <c r="H13" t="s">
@@ -933,16 +941,16 @@
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="15" t="s">
         <v>50</v>
       </c>
       <c r="H14" t="s">
@@ -950,16 +958,16 @@
       </c>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="15" t="s">
         <v>49</v>
       </c>
       <c r="H15" t="s">
@@ -967,14 +975,14 @@
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="15" t="s">
         <v>51</v>
       </c>
       <c r="H16" t="s">
@@ -982,16 +990,16 @@
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="14" t="s">
         <v>81</v>
       </c>
       <c r="H17" t="s">
@@ -999,230 +1007,230 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="15" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="20"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="20"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="20"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="20"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" spans="2:8">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="20"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="15" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="15" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="20"/>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="20"/>
+      <c r="E33" s="15"/>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="20"/>
+      <c r="E34" s="15"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="15" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add globbing (--include, --exclude)
</commit_message>
<xml_diff>
--- a/Grep Options Analysis.xlsx
+++ b/Grep Options Analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>b</t>
   </si>
@@ -339,13 +339,40 @@
   </si>
   <si>
     <t>recursive+symlink</t>
+  </si>
+  <si>
+    <t>GREPL SPECIFIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --save</t>
+  </si>
+  <si>
+    <t>replace and save</t>
+  </si>
+  <si>
+    <t>replace (preview)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --var &lt;name&gt; &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>regex template variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --group</t>
+  </si>
+  <si>
+    <t>group files by context</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +429,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -454,8 +488,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -492,10 +525,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -516,7 +550,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -534,10 +567,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -816,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H35"/>
+  <dimension ref="B2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,50 +862,57 @@
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="C2" s="20" t="s">
+    <row r="2" spans="2:9">
+      <c r="C2" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="2:8">
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:9">
       <c r="C3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:8">
-      <c r="C4" s="19" t="s">
+    <row r="4" spans="2:9">
+      <c r="C4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="C5" s="22" t="s">
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="C5" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="C6" s="21" t="s">
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="C6" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="C7" s="23" t="s">
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="C7" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="23"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="H9" t="s">
+      <c r="D7" s="22"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="G9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="2:8">
+      <c r="H9" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
@@ -884,11 +925,17 @@
       <c r="E10" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="G10" s="15" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="H10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
       <c r="B11" s="11" t="s">
         <v>0</v>
       </c>
@@ -901,11 +948,17 @@
       <c r="E11" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="15" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="H11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
       <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
@@ -915,15 +968,21 @@
       <c r="D12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>76</v>
       </c>
       <c r="F12" s="13"/>
-      <c r="H12" s="15" t="s">
+      <c r="G12" s="15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13" s="12" t="s">
         <v>3</v>
       </c>
@@ -933,18 +992,24 @@
       <c r="D13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>93</v>
       </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
       <c r="H13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
+        <v>112</v>
+      </c>
+      <c r="I13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -953,15 +1018,15 @@
       <c r="E14" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" s="23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:9">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -970,11 +1035,11 @@
       <c r="E15" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:9">
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
@@ -985,11 +1050,11 @@
       <c r="E16" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:7">
       <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
@@ -1002,11 +1067,11 @@
       <c r="E17" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17" s="23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:7">
       <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
@@ -1019,11 +1084,12 @@
       <c r="E18" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:7">
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +1099,7 @@
       </c>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:7">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
@@ -1043,11 +1109,11 @@
       </c>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:7">
       <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D21" s="8" t="s">
@@ -1057,7 +1123,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:7">
       <c r="B22" s="8" t="s">
         <v>12</v>
       </c>
@@ -1069,7 +1135,7 @@
       </c>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:7">
       <c r="B23" s="11" t="s">
         <v>13</v>
       </c>
@@ -1081,7 +1147,7 @@
       </c>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:7">
       <c r="B24" s="8" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1159,7 @@
       </c>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:7">
       <c r="B25" s="3" t="s">
         <v>15</v>
       </c>
@@ -1105,7 +1171,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:7">
       <c r="B26" s="8" t="s">
         <v>16</v>
       </c>
@@ -1117,22 +1183,22 @@
       </c>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:7">
       <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>100</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="16" t="s">
         <v>104</v>
       </c>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:7">
       <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
@@ -1144,7 +1210,7 @@
       </c>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:7">
       <c r="B29" s="9" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +1222,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:7">
       <c r="B30" s="11" t="s">
         <v>20</v>
       </c>
@@ -1170,7 +1236,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:7">
       <c r="B31" s="4" t="s">
         <v>21</v>
       </c>
@@ -1184,7 +1250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:7">
       <c r="B32" s="4" t="s">
         <v>22</v>
       </c>

</xml_diff>